<commit_message>
CreateItem Method modify to make copis of the model and update the ccreation time  on sources.
</commit_message>
<xml_diff>
--- a/schedule_data.xlsx
+++ b/schedule_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uxia\Documents\GitHub\PyFlow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PyFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D5F37F-3F7F-4B24-8811-471FAF0BF6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182DAFDF-E683-42A9-A114-5AA307839018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3912" yWindow="2256" windowWidth="17280" windowHeight="8880" xr2:uid="{A34F26A0-950C-4EF8-94B0-1F4CA0DEB41A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A34F26A0-950C-4EF8-94B0-1F4CA0DEB41A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,54 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Item1</t>
-  </si>
-  <si>
-    <t>Item2</t>
-  </si>
-  <si>
-    <t>Item3</t>
-  </si>
-  <si>
-    <t>Item4</t>
-  </si>
-  <si>
-    <t>Item5</t>
-  </si>
-  <si>
-    <t>10.5</t>
-  </si>
-  <si>
-    <t>20.75</t>
-  </si>
-  <si>
-    <t>30.5</t>
-  </si>
-  <si>
-    <t>Item6</t>
-  </si>
-  <si>
-    <t>Item7</t>
-  </si>
-  <si>
-    <t>Item8</t>
-  </si>
-  <si>
-    <t>Item9</t>
-  </si>
-  <si>
-    <t>Item10</t>
-  </si>
-  <si>
-    <t>35.25</t>
-  </si>
-  <si>
-    <t>45.5</t>
-  </si>
-  <si>
-    <t>50.75</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>item2</t>
+  </si>
+  <si>
+    <t>item3</t>
+  </si>
+  <si>
+    <t>item4</t>
+  </si>
+  <si>
+    <t>javi</t>
+  </si>
+  <si>
+    <t>pedro</t>
+  </si>
+  <si>
+    <t>cris</t>
+  </si>
+  <si>
+    <t>fran</t>
   </si>
 </sst>
 </file>
@@ -133,12 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +130,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -473,129 +446,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87ED9BA-7A41-4B92-8F52-45D5F37A171A}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1">
         <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>40</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>55</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H14" s="1"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Schedule source completed and items cna be used as models.
</commit_message>
<xml_diff>
--- a/schedule_data.xlsx
+++ b/schedule_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PyFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182DAFDF-E683-42A9-A114-5AA307839018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A633C9-EDD4-41D1-8BBD-382709FCCBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A34F26A0-950C-4EF8-94B0-1F4CA0DEB41A}"/>
   </bookViews>
@@ -50,16 +50,16 @@
     <t>item4</t>
   </si>
   <si>
-    <t>javi</t>
-  </si>
-  <si>
-    <t>pedro</t>
-  </si>
-  <si>
-    <t>cris</t>
-  </si>
-  <si>
-    <t>fran</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -470,13 +470,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -484,13 +484,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated Schedule Source to support also .data and .csv files.
Files format is updated to support label creation on items from file.
</commit_message>
<xml_diff>
--- a/schedule_data.xlsx
+++ b/schedule_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PyFlow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpern\Documents\GitHub\PyFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A633C9-EDD4-41D1-8BBD-382709FCCBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74357CA-EFF6-4587-9069-4DA4D2A5F07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A34F26A0-950C-4EF8-94B0-1F4CA0DEB41A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{A34F26A0-950C-4EF8-94B0-1F4CA0DEB41A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>item1</t>
-  </si>
-  <si>
-    <t>item2</t>
-  </si>
-  <si>
-    <t>item3</t>
-  </si>
-  <si>
-    <t>item4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>A</t>
   </si>
@@ -60,6 +48,21 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Plancha</t>
   </si>
 </sst>
 </file>
@@ -446,75 +449,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87ED9BA-7A41-4B92-8F52-45D5F37A171A}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>10</v>
+      <c r="A1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H14" s="1"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>